<commit_message>
add StreamImpactItem to account for impacts associate with WasteStreams'
</commit_message>
<xml_diff>
--- a/sanitation/data/_impact_item.xlsx
+++ b/sanitation/data/_impact_item.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bfca01abaf64aab7/Coding/sanitation_Yalin/sanitation/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="134" documentId="8_{935E0A0B-8DD3-6742-99D3-41177F9390EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{87CB4B4C-DA22-B945-965D-37956C8A22CB}"/>
+  <xr:revisionPtr revIDLastSave="138" documentId="8_{935E0A0B-8DD3-6742-99D3-41177F9390EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BECA1650-402B-F04F-BB67-DC36039BAF5C}"/>
   <bookViews>
     <workbookView xWindow="9380" yWindow="2260" windowWidth="27240" windowHeight="16440" xr2:uid="{BD97E243-0BB4-3F42-9EBC-00D49E7EE019}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="28">
   <si>
     <t>ecoinvent 3</t>
   </si>
@@ -80,9 +80,6 @@
     <t>expected</t>
   </si>
   <si>
-    <t>material</t>
-  </si>
-  <si>
     <t>functional_unit</t>
   </si>
   <si>
@@ -101,15 +98,9 @@
     <t>ID</t>
   </si>
   <si>
-    <t>kind</t>
-  </si>
-  <si>
     <t>Concrete</t>
   </si>
   <si>
-    <t>activity</t>
-  </si>
-  <si>
     <t>unit</t>
   </si>
   <si>
@@ -120,9 +111,6 @@
   </si>
   <si>
     <t>Brick</t>
-  </si>
-  <si>
-    <t>transportation</t>
   </si>
   <si>
     <t>tonne*km</t>
@@ -525,160 +513,120 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66379A7A-E84B-1346-816F-577916F7D6A6}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="B4" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>18</v>
       </c>
-      <c r="B9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>19</v>
-      </c>
       <c r="B10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -702,10 +650,10 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>13</v>
@@ -729,7 +677,7 @@
         <v>Excavation</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C2" s="6">
         <v>0.53</v>
@@ -753,7 +701,7 @@
         <v>Brick</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C3" s="7">
         <v>0.28000000000000003</v>
@@ -777,7 +725,7 @@
         <v>Cement</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C4" s="7">
         <v>1.08</v>
@@ -801,7 +749,7 @@
         <v>Concrete</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C5" s="4">
         <v>300</v>
@@ -825,7 +773,7 @@
         <v>Gravel</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C6" s="6">
         <v>1.4999999999999999E-2</v>
@@ -849,7 +797,7 @@
         <v>Plastic</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C7" s="6">
         <v>1.97</v>
@@ -873,7 +821,7 @@
         <v>Sand</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C8" s="6">
         <v>1.2E-2</v>
@@ -897,7 +845,7 @@
         <v>StainlessSteel</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C9" s="6">
         <v>4.33</v>
@@ -921,7 +869,7 @@
         <v>StainlessSteelSheet</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C10" s="6">
         <v>0.65</v>
@@ -945,7 +893,7 @@
         <v>Steel</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C11" s="6">
         <v>2.5499999999999998</v>
@@ -969,7 +917,7 @@
         <v>Wood</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C12" s="6">
         <v>197</v>
@@ -993,7 +941,7 @@
         <v>Trucking</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C13" s="4">
         <v>0.19400000000000001</v>
@@ -1008,7 +956,7 @@
         <v>1</v>
       </c>
       <c r="G13" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -1039,10 +987,10 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>13</v>
@@ -1066,7 +1014,7 @@
         <v>Excavation</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C2" s="6">
         <v>7.3000000000000007</v>
@@ -1090,7 +1038,7 @@
         <v>Brick</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C3" s="7">
         <v>4.8000000000000007</v>
@@ -1114,7 +1062,7 @@
         <v>Cement</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C4" s="7">
         <v>12.8</v>
@@ -1138,7 +1086,7 @@
         <v>Concrete</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
@@ -1156,7 +1104,7 @@
         <v>Gravel</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
@@ -1174,7 +1122,7 @@
         <v>Plastic</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
@@ -1192,7 +1140,7 @@
         <v>Sand</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
@@ -1210,7 +1158,7 @@
         <v>StainlessSteel</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C9" s="6">
         <v>45.3</v>
@@ -1234,7 +1182,7 @@
         <v>StainlessSteelSheet</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C10" s="6">
         <v>8.5</v>
@@ -1258,7 +1206,7 @@
         <v>Steel</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C11" s="6">
         <v>27.5</v>
@@ -1282,7 +1230,7 @@
         <v>Wood</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C12" s="6">
         <v>1972</v>
@@ -1306,7 +1254,7 @@
         <v>Trucking</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C13" s="6">
         <v>3.94</v>

</xml_diff>

<commit_message>
complete LCA design, try to fix Travis CI
</commit_message>
<xml_diff>
--- a/sanitation/data/_impact_item.xlsx
+++ b/sanitation/data/_impact_item.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bfca01abaf64aab7/Coding/sanitation_Yalin/sanitation/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="138" documentId="8_{935E0A0B-8DD3-6742-99D3-41177F9390EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BECA1650-402B-F04F-BB67-DC36039BAF5C}"/>
+  <xr:revisionPtr revIDLastSave="141" documentId="8_{935E0A0B-8DD3-6742-99D3-41177F9390EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6ED48F83-EA29-C847-9B9A-FC988CD045AA}"/>
   <bookViews>
-    <workbookView xWindow="9380" yWindow="2260" windowWidth="27240" windowHeight="16440" xr2:uid="{BD97E243-0BB4-3F42-9EBC-00D49E7EE019}"/>
+    <workbookView xWindow="9380" yWindow="2260" windowWidth="27240" windowHeight="16440" activeTab="2" xr2:uid="{BD97E243-0BB4-3F42-9EBC-00D49E7EE019}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="2" r:id="rId1"/>
@@ -515,7 +515,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66379A7A-E84B-1346-816F-577916F7D6A6}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -975,8 +975,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92BA73E1-0EB2-7B4F-9241-A5B8DBA36260}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1088,9 +1088,15 @@
       <c r="B5" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
+      <c r="C5" s="4">
+        <v>0</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0</v>
+      </c>
       <c r="F5" s="4" t="s">
         <v>1</v>
       </c>
@@ -1106,9 +1112,15 @@
       <c r="B6" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
+      <c r="C6" s="4">
+        <v>0</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0</v>
+      </c>
       <c r="F6" s="4" t="s">
         <v>1</v>
       </c>
@@ -1124,9 +1136,15 @@
       <c r="B7" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
+      <c r="C7" s="4">
+        <v>0</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0</v>
+      </c>
       <c r="F7" s="4" t="s">
         <v>1</v>
       </c>
@@ -1142,9 +1160,15 @@
       <c r="B8" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
+      <c r="C8" s="4">
+        <v>0</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0</v>
+      </c>
       <c r="F8" s="4" t="s">
         <v>1</v>
       </c>

</xml_diff>